<commit_message>
adding abstraction,encapsulation and inheritence
</commit_message>
<xml_diff>
--- a/excel.xlsx
+++ b/excel.xlsx
@@ -39,25 +39,25 @@
     <t>Password</t>
   </si>
   <si>
-    <t>abhijeet</t>
-  </si>
-  <si>
-    <t>singh</t>
+    <t>Abhijeet</t>
+  </si>
+  <si>
+    <t>Singh</t>
   </si>
   <si>
     <t>abhijeetsinghraj2345@gmail.com</t>
   </si>
   <si>
-    <t>+918698567256</t>
+    <t>+918698567733</t>
   </si>
   <si>
     <t>Male</t>
   </si>
   <si>
-    <t>2006-2-25</t>
-  </si>
-  <si>
-    <t>111111111111111</t>
+    <t>1997-12-22</t>
+  </si>
+  <si>
+    <t>abhijeet1234</t>
   </si>
 </sst>
 </file>
@@ -398,7 +398,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="A1:G5"/>
+      <selection activeCell="A5" sqref="A1:G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.3" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Handling PermissionError with try-except
</commit_message>
<xml_diff>
--- a/excel.xlsx
+++ b/excel.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="8015" windowWidth="14808" xWindow="245" yWindow="109"/>
+    <workbookView xWindow="245" yWindow="109" windowWidth="14808" windowHeight="8015"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>First Name</t>
   </si>
@@ -63,20 +63,19 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -92,15 +91,21 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleMedium9" defaultTableStyle="TableStyleMedium2"/>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -390,29 +395,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A1:G5"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.3" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
   <cols>
-    <col customWidth="1" max="2" min="1" width="20"/>
-    <col customWidth="1" max="2" min="2" width="20"/>
-    <col customWidth="1" max="3" min="3" width="30"/>
-    <col customWidth="1" max="4" min="4" width="20"/>
-    <col customWidth="1" max="5" min="5" width="10"/>
-    <col customWidth="1" max="7" min="6" width="30"/>
-    <col customWidth="1" max="7" min="7" width="30"/>
+    <col min="1" max="2" width="20" customWidth="1"/>
+    <col min="3" max="3" width="30" customWidth="1"/>
+    <col min="4" max="4" width="20" customWidth="1"/>
+    <col min="5" max="5" width="10" customWidth="1"/>
+    <col min="6" max="7" width="30" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -435,7 +434,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -459,42 +458,30 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.3"/>
+  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
   <sheetData/>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.3"/>
+  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
   <sheetData/>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>